<commit_message>
download button appears when make attendance is clicked
</commit_message>
<xml_diff>
--- a/Attendance/sheet_2.xlsx
+++ b/Attendance/sheet_2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>for month 1</t>
+          <t>2021/1/19</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -458,30 +458,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Muskan Vaswan</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2021-01-15 09:20:00.484737+00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Muskan Vaswan</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2021-01-15 11:02:48.016808+00:00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>